<commit_message>
updating dirty data samples
</commit_message>
<xml_diff>
--- a/sample/dirty.xlsx
+++ b/sample/dirty.xlsx
@@ -12,24 +12,19 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6770"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="dirty" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>Points Scored (winning)</t>
-  </si>
-  <si>
-    <t>Points Scored (losing)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+  <si>
+    <t xml:space="preserve">Winning Team </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Losing Team</t>
   </si>
   <si>
     <t>Winning Team % of Total</t>
@@ -41,12 +36,6 @@
     <t># Penalties</t>
   </si>
   <si>
-    <t xml:space="preserve">Winning Team </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Losing Team</t>
-  </si>
-  <si>
     <t>Narwhals</t>
   </si>
   <si>
@@ -69,13 +58,43 @@
   </si>
   <si>
     <t>Woodpeckers</t>
+  </si>
+  <si>
+    <t>Referee</t>
+  </si>
+  <si>
+    <t>Einstein</t>
+  </si>
+  <si>
+    <t>Newton</t>
+  </si>
+  <si>
+    <t>Galilei</t>
+  </si>
+  <si>
+    <t>Curie</t>
+  </si>
+  <si>
+    <t>Maxwell</t>
+  </si>
+  <si>
+    <t>Darwin</t>
+  </si>
+  <si>
+    <t>Lamarr</t>
+  </si>
+  <si>
+    <t>Points Scored (winning team)</t>
+  </si>
+  <si>
+    <t>Points Scored (losing team)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,16 +102,316 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -100,17 +419,205 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -388,32 +895,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6328125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -424,13 +925,19 @@
       <c r="H1" t="s">
         <v>4</v>
       </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>11</v>
@@ -439,8 +946,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="1">
-        <f>C3/SUM(C3:D3)</f>
-        <v>0.6470588235294118</v>
+        <v>0.65</v>
       </c>
       <c r="F3">
         <v>10</v>
@@ -448,13 +954,19 @@
       <c r="H3">
         <v>2</v>
       </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>12</v>
@@ -463,7 +975,6 @@
         <v>4</v>
       </c>
       <c r="E4" s="1">
-        <f>C4/SUM(C4:D4)</f>
         <v>0.75</v>
       </c>
       <c r="F4">
@@ -472,13 +983,19 @@
       <c r="H4">
         <v>1</v>
       </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>7</v>
@@ -486,8 +1003,7 @@
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6" s="2">
-        <f>C6/SUM(C6:D6)</f>
+      <c r="E6" s="1">
         <v>1</v>
       </c>
       <c r="F6">
@@ -496,13 +1012,16 @@
       <c r="H6">
         <v>3</v>
       </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7">
         <v>15</v>
@@ -510,19 +1029,23 @@
       <c r="D7">
         <v>14</v>
       </c>
-      <c r="E7" s="2">
-        <f>C7/SUM(C7:D7)</f>
-        <v>0.51724137931034486</v>
+      <c r="E7" s="1">
+        <v>0.52</v>
       </c>
       <c r="F7">
         <v>17</v>
       </c>
       <c r="H7">
         <v>2</v>
+      </c>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update readme and sample data to include excel_numeric_to_dates example
</commit_message>
<xml_diff>
--- a/sample/dirty.xlsx
+++ b/sample/dirty.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t xml:space="preserve">Winning Team </t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Points Scored (losing team)</t>
+  </si>
+  <si>
+    <t>Match Date</t>
   </si>
 </sst>
 </file>
@@ -571,9 +574,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -895,15 +899,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="11" max="11" width="9.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -931,8 +938,11 @@
       <c r="J1" t="s">
         <v>13</v>
       </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -960,8 +970,11 @@
       <c r="J3" t="s">
         <v>15</v>
       </c>
+      <c r="K3" s="2">
+        <v>42461</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -989,8 +1002,14 @@
       <c r="J4" t="s">
         <v>17</v>
       </c>
+      <c r="K4" s="2">
+        <v>42464</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1015,8 +1034,11 @@
       <c r="I6" t="s">
         <v>18</v>
       </c>
+      <c r="K6" s="2">
+        <v>42459</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1043,6 +1065,9 @@
       </c>
       <c r="J7" t="s">
         <v>20</v>
+      </c>
+      <c r="K7" s="2">
+        <v>42467</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix % formatting issue in sample data
</commit_message>
<xml_diff>
--- a/sample/dirty.xlsx
+++ b/sample/dirty.xlsx
@@ -576,8 +576,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -902,7 +902,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="E3" sqref="E3:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -955,7 +955,7 @@
       <c r="D3">
         <v>6</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
         <v>0.65</v>
       </c>
       <c r="F3">
@@ -970,7 +970,7 @@
       <c r="J3" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="1">
         <v>42461</v>
       </c>
     </row>
@@ -987,7 +987,7 @@
       <c r="D4">
         <v>4</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="2">
         <v>0.75</v>
       </c>
       <c r="F4">
@@ -1002,12 +1002,13 @@
       <c r="J4" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="1">
         <v>42464</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="K5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -1022,7 +1023,7 @@
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="2">
         <v>1</v>
       </c>
       <c r="F6">
@@ -1034,7 +1035,7 @@
       <c r="I6" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="1">
         <v>42459</v>
       </c>
     </row>
@@ -1051,7 +1052,7 @@
       <c r="D7">
         <v>14</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="2">
         <v>0.52</v>
       </c>
       <c r="F7">
@@ -1066,7 +1067,7 @@
       <c r="J7" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="1">
         <v>42467</v>
       </c>
     </row>

</xml_diff>